<commit_message>
This code is working
</commit_message>
<xml_diff>
--- a/Entries.xlsx
+++ b/Entries.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="udacity.com" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="instagram.com" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gla.ac.uk" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="slu.edu" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,25 +426,61 @@
     <row r="1">
       <c r="B1" t="inlineStr">
         <is>
-          <t>Cloudflare</t>
+          <t>Cloudflare DOH</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>Mozilla Cloudflare</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>Google DOH</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Quad9</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Comcast</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Adguard</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Cloudflare DNS</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>OpenDNS</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Vodafone Idea India</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>Baidu(China)</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Shenzen(China)</t>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Google DNS</t>
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -452,18 +488,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.05529379844665527</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>$$$$</t>
-        </is>
+        <v>0.1033837795257568</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.6198141574859619</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4683408737182617</v>
+        <v>0.1586830615997314</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3022820949554443</v>
+        <v>0.1770989894866943</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6077830791473389</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1257741451263428</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.03684473037719727</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.04202795028686523</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.4674160480499268</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5356969833374023</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.02459907531738281</v>
       </c>
     </row>
     <row r="4">
@@ -474,286 +529,119 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>id 9409
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-udacity.com. IN NS
-;ANSWER
-udacity.com. 170080 IN NS ns-1014.awsdns-62.net.
-udacity.com. 170080 IN NS ns-1109.awsdns-10.org.
-udacity.com. 170080 IN NS ns-13.awsdns-01.com.
-udacity.com. 170080 IN NS ns-1549.awsdns-01.co.uk.
-;AUTHORITY
-;ADDITIONAL</t>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 30378
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              476     IN      A       130.209.16.93</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$$$$</t>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 30378
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              475     IN      A       130.209.16.93</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>id 9409
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-udacity.com. IN NS
-;ANSWER
-udacity.com. 172769 IN NS ns-1014.awsdns-62.net.
-udacity.com. 172769 IN NS ns-1109.awsdns-10.org.
-udacity.com. 172769 IN NS ns-1549.awsdns-01.co.uk.
-udacity.com. 172769 IN NS ns-13.awsdns-01.com.
-;AUTHORITY
-;ADDITIONAL
-ns-13.awsdns-01.com. 68512 IN A 205.251.192.13
-ns-1014.awsdns-62.net. 66585 IN A 205.251.195.246
-ns-1109.awsdns-10.org. 66849 IN A 205.251.196.85
-ns-1549.awsdns-01.co.uk. 66919 IN A 205.251.198.13</t>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 30378
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              599     IN      A       130.209.16.93</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>id 9409
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-udacity.com. IN NS
-;ANSWER
-udacity.com. 84636 IN NS ns-1109.awsdns-10.org.
-udacity.com. 84636 IN NS ns-1549.awsdns-01.co.uk.
-udacity.com. 84636 IN NS ns-13.awsdns-01.com.
-udacity.com. 84636 IN NS ns-1014.awsdns-62.net.
-;AUTHORITY
-;ADDITIONAL
-ns-13.awsdns-01.com. 20735 IN A 205.251.192.13</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Cloudflare</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Google</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Baidu(China)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Shenzen(China)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.08156800270080566</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>$$$$</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>0.5410821437835693</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.4090580940246582</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Result</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>id 42966
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-udacity.com. IN NS
-;ANSWER
-udacity.com. 169896 IN NS ns-1014.awsdns-62.net.
-udacity.com. 169896 IN NS ns-1109.awsdns-10.org.
-udacity.com. 169896 IN NS ns-13.awsdns-01.com.
-udacity.com. 169896 IN NS ns-1549.awsdns-01.co.uk.
-;AUTHORITY
-;ADDITIONAL</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>$$$$</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>id 42966
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-udacity.com. IN NS
-;ANSWER
-udacity.com. 172585 IN NS ns-13.awsdns-01.com.
-udacity.com. 172585 IN NS ns-1109.awsdns-10.org.
-udacity.com. 172585 IN NS ns-1549.awsdns-01.co.uk.
-udacity.com. 172585 IN NS ns-1014.awsdns-62.net.
-;AUTHORITY
-;ADDITIONAL
-ns-13.awsdns-01.com. 68328 IN A 205.251.192.13
-ns-1014.awsdns-62.net. 66401 IN A 205.251.195.246
-ns-1109.awsdns-10.org. 66665 IN A 205.251.196.85
-ns-1549.awsdns-01.co.uk. 66735 IN A 205.251.198.13</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>id 42966
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-udacity.com. IN NS
-;ANSWER
-udacity.com. 84451 IN NS ns-13.awsdns-01.com.
-udacity.com. 84451 IN NS ns-1109.awsdns-10.org.
-udacity.com. 84451 IN NS ns-1014.awsdns-62.net.
-udacity.com. 84451 IN NS ns-1549.awsdns-01.co.uk.
-;AUTHORITY
-;ADDITIONAL
-ns-13.awsdns-01.com. 20550 IN A 205.251.192.13</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Cloudflare</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Google</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Baidu(China)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Shenzen(China)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10"/>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0.06363630294799805</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>$$$$</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>0.3946611881256104</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.3377749919891357</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Result</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>id 53445
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-udacity.com. IN NS
-;ANSWER
-udacity.com. 169480 IN NS ns-1014.awsdns-62.net.
-udacity.com. 169480 IN NS ns-1109.awsdns-10.org.
-udacity.com. 169480 IN NS ns-13.awsdns-01.com.
-udacity.com. 169480 IN NS ns-1549.awsdns-01.co.uk.
-;AUTHORITY
-;ADDITIONAL</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>$$$$</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>id 53445
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-udacity.com. IN NS
-;ANSWER
-udacity.com. 172169 IN NS ns-1549.awsdns-01.co.uk.
-udacity.com. 172169 IN NS ns-13.awsdns-01.com.
-udacity.com. 172169 IN NS ns-1109.awsdns-10.org.
-udacity.com. 172169 IN NS ns-1014.awsdns-62.net.
-;AUTHORITY
-;ADDITIONAL
-ns-13.awsdns-01.com. 67912 IN A 205.251.192.13
-ns-1014.awsdns-62.net. 65985 IN A 205.251.195.246
-ns-1109.awsdns-10.org. 66249 IN A 205.251.196.85
-ns-1549.awsdns-01.co.uk. 66319 IN A 205.251.198.13</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>id 53445
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-udacity.com. IN NS
-;ANSWER
-udacity.com. 84036 IN NS ns-1109.awsdns-10.org.
-udacity.com. 84036 IN NS ns-1014.awsdns-62.net.
-udacity.com. 84036 IN NS ns-13.awsdns-01.com.
-udacity.com. 84036 IN NS ns-1549.awsdns-01.co.uk.
-;AUTHORITY
-;ADDITIONAL
-ns-13.awsdns-01.com. 20135 IN A 205.251.192.13</t>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 30378
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              473     IN      A       130.209.16.93</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 0
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              600     IN      A       130.209.16.93</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 30378
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              600     IN      A       130.209.16.93</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 30378
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              474     IN      A       130.209.16.93</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 30378
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              474     IN      A       130.209.16.93</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 30378
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              600     IN      A       130.209.16.93</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 30378
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 3, ADDITIONAL: 2
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              475     IN      A       130.209.16.93
+;; AUTHORITY SECTION:
+gla.ac.uk.              293013  IN      NS      dns1.gla.ac.uk.
+gla.ac.uk.              293013  IN      NS      dns2.gla.ac.uk.
+gla.ac.uk.              293013  IN      NS      dns0.gla.ac.uk.
+;; ADDITIONAL SECTION:
+dns1.gla.ac.uk.         3461    IN      AAAA    2001:630:40:40::10
+dns2.gla.ac.uk.         3461    IN      AAAA    2001:630:40:40::12</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 30378
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;gla.ac.uk.                     IN      A
+;; ANSWER SECTION:
+gla.ac.uk.              203     IN      A       130.209.16.93</t>
         </is>
       </c>
     </row>
@@ -768,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -779,22 +667,57 @@
     <row r="1">
       <c r="B1" t="inlineStr">
         <is>
-          <t>Cloudflare</t>
+          <t>Cloudflare DOH</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>Mozilla Cloudflare</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>Google DOH</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Quad9</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Comcast</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Adguard</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Cloudflare DNS</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>OpenDNS</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Vodafone Idea India</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>Baidu(China)</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Shenzen(China)</t>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Google DNS</t>
         </is>
       </c>
     </row>
@@ -805,18 +728,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0969388484954834</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>$$$$</t>
-        </is>
+        <v>0.117664098739624</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.06178498268127441</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3327281475067139</v>
+        <v>0.09466314315795898</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3180298805236816</v>
+        <v>0.04030084609985352</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.7797970771789551</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.6454668045043945</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.003655910491943359</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.2325811386108398</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.8008787631988525</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.3917508125305176</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.04346323013305664</v>
       </c>
     </row>
     <row r="4">
@@ -827,64 +769,122 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>id 57078
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-instagram.com. IN NS
-;ANSWER
-instagram.com. 170514 IN NS ns-1349.awsdns-40.org.
-instagram.com. 170514 IN NS ns-2016.awsdns-60.co.uk.
-instagram.com. 170514 IN NS ns-384.awsdns-48.com.
-instagram.com. 170514 IN NS ns-868.awsdns-44.net.
-;AUTHORITY
-;ADDITIONAL</t>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 38724
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                88      IN      A       173.213.236.59</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$$$$</t>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 38724
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                88      IN      A       173.213.236.59</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>id 57078
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-instagram.com. IN NS
-;ANSWER
-instagram.com. 66359 IN NS ns-2016.awsdns-60.co.uk.
-instagram.com. 66359 IN NS ns-1349.awsdns-40.org.
-instagram.com. 66359 IN NS ns-868.awsdns-44.net.
-instagram.com. 66359 IN NS ns-384.awsdns-48.com.
-;AUTHORITY
-;ADDITIONAL
-ns-384.awsdns-48.com. 37240 IN A 205.251.193.128
-ns-868.awsdns-44.net. 66529 IN A 205.251.195.100
-ns-1349.awsdns-40.org. 66509 IN A 205.251.197.69
-ns-2016.awsdns-60.co.uk. 66517 IN A 205.251.199.224</t>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 38724
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                90      IN      A       173.213.236.59</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>id 57078
-opcode QUERY
-rcode NOERROR
-flags QR RD RA
-;QUESTION
-instagram.com. IN NS
-;ANSWER
-instagram.com. 41108 IN NS ns-868.awsdns-44.net.
-instagram.com. 41108 IN NS ns-2016.awsdns-60.co.uk.
-instagram.com. 41108 IN NS ns-1349.awsdns-40.org.
-instagram.com. 41108 IN NS ns-384.awsdns-48.com.
-;AUTHORITY
-;ADDITIONAL
-ns-384.awsdns-48.com. 20317 IN A 205.251.193.128
-ns-868.awsdns-44.net. 125821 IN A 205.251.195.100</t>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 38724
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                88      IN      A       173.213.236.59</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 0
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                88      IN      A       173.213.236.59</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 38724
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                300     IN      A       173.213.236.59</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 38724
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                87      IN      A       173.213.236.59</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 38724
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                300     IN      A       173.213.236.59</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 38724
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                300     IN      A       173.213.236.59</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 38724
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 4, ADDITIONAL: 4
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                300     IN      A       173.213.236.59
+;; AUTHORITY SECTION:
+slu.edu.                97926   IN      NS      ns2.g02.cfdns.biz.
+slu.edu.                97926   IN      NS      ns4.g02.cfdns.co.uk.
+slu.edu.                97926   IN      NS      ns1.g02.cfdns.net.
+slu.edu.                97926   IN      NS      ns3.g02.cfdns.info.
+;; ADDITIONAL SECTION:
+ns1.g02.cfdns.net.      8310    IN      A       199.73.82.2
+ns2.g02.cfdns.biz.      21049   IN      A       199.73.83.2
+ns3.g02.cfdns.info.     46908   IN      A       204.138.102.2
+ns4.g02.cfdns.co.uk.    46906   IN      A       192.188.176.2</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>;; -&gt;&gt;HEADER&lt;&lt;- opcode: QUERY, status: NOERROR, id: 38724
+;; flags: qr rd ra; QUERY: 1, ANSWER: 1, AUTHORITY: 0, ADDITIONAL: 0
+;; QUESTION SECTION:
+;slu.edu.                       IN      A
+;; ANSWER SECTION:
+slu.edu.                299     IN      A       173.213.236.59</t>
         </is>
       </c>
     </row>

</xml_diff>